<commit_message>
export file mẫu product
</commit_message>
<xml_diff>
--- a/src/main/resources/static/fileMau/fileMauVoucher.xlsx
+++ b/src/main/resources/static/fileMau/fileMauVoucher.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\DATN\DATN_BE_2003Shoes\src\main\resources\static\fileMau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6113D4D-EFE5-41B2-9AD6-D3B5C23E4104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4D489A-6BA1-4794-B174-CDD64369E1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10080" xr2:uid="{E5B39717-D5A6-446F-B264-D4DBCAC40ED0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E5B39717-D5A6-446F-B264-D4DBCAC40ED0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,8 +353,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">)
-</t>
+      <t>)</t>
     </r>
   </si>
 </sst>
@@ -756,8 +755,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>